<commit_message>
Added population tool for Rick
</commit_message>
<xml_diff>
--- a/Dijkstra/main/Aggregated_nodes.xlsx
+++ b/Dijkstra/main/Aggregated_nodes.xlsx
@@ -4731,7 +4731,7 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>238</v>
+        <v>419</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -4739,7 +4739,7 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>238</v>
+        <v>419</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -4787,7 +4787,7 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>238</v>
+        <v>419</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -4795,7 +4795,7 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>238</v>
+        <v>419</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -4803,7 +4803,7 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>238</v>
+        <v>419</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -4811,7 +4811,7 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>238</v>
+        <v>419</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -4819,7 +4819,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>238</v>
+        <v>419</v>
       </c>
     </row>
     <row r="239" spans="1:2">

</xml_diff>